<commit_message>
update to dashboard and overall layout
</commit_message>
<xml_diff>
--- a/backend/jacfit_template.xlsx
+++ b/backend/jacfit_template.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Chin ups</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Shuttle Runs</t>
+          <t>Sprint 40y</t>
         </is>
       </c>
     </row>
@@ -481,7 +476,6 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -499,25 +493,6 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Julie</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Piers</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>